<commit_message>
- documentation updated (connectors reference)
</commit_message>
<xml_diff>
--- a/V2/DOC/ConnectorsReference.xlsx
+++ b/V2/DOC/ConnectorsReference.xlsx
@@ -758,49 +758,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -839,18 +800,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -860,10 +844,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1659,8 +1658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1684,955 +1683,949 @@
   <sheetData>
     <row r="1" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:16" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="57"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="J2" s="5" t="s">
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="51"/>
+      <c r="J2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="7"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="51"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="10" t="s">
+      <c r="B3" s="59"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="60" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="J3" s="53" t="s">
+      <c r="H3" s="61"/>
+      <c r="J3" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="54"/>
-      <c r="L3" s="53" t="s">
+      <c r="K3" s="46"/>
+      <c r="L3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="54"/>
-      <c r="N3" s="58" t="s">
+      <c r="M3" s="46"/>
+      <c r="N3" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="59"/>
-      <c r="P3" s="60"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="54"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="14" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="14" t="s">
+      <c r="E4" s="44"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="J4" s="12" t="s">
+      <c r="H4" s="44"/>
+      <c r="J4" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="13"/>
-      <c r="L4" s="12" t="s">
+      <c r="K4" s="48"/>
+      <c r="L4" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="M4" s="13"/>
-      <c r="N4" s="12" t="s">
+      <c r="M4" s="48"/>
+      <c r="N4" s="47" t="s">
         <v>45</v>
       </c>
       <c r="O4" s="55"/>
-      <c r="P4" s="13"/>
+      <c r="P4" s="48"/>
     </row>
     <row r="5" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="16" t="s">
+      <c r="C5" s="5"/>
+      <c r="D5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="16" t="s">
+      <c r="L5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="17" t="s">
+      <c r="M5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="56" t="s">
+      <c r="O5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="17" t="s">
+      <c r="P5" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21">
+      <c r="A6" s="8">
         <v>1</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="27" t="s">
+      <c r="F6" s="13"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="8">
         <v>1</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="8">
         <v>1</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="21">
+      <c r="N6" s="8">
         <v>1</v>
       </c>
-      <c r="O6" s="28" t="s">
+      <c r="O6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="P6" s="61">
+      <c r="P6" s="41">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21">
+      <c r="A7" s="8">
         <v>2</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="27" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="26"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="25" t="s">
+      <c r="F7" s="13"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="8">
         <v>2</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="21">
+      <c r="L7" s="8">
         <v>2</v>
       </c>
-      <c r="M7" s="28" t="s">
+      <c r="M7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="N7" s="21">
+      <c r="N7" s="8">
         <v>2</v>
       </c>
-      <c r="O7" s="28" t="s">
+      <c r="O7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="61">
+      <c r="P7" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="8">
         <v>3</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="32" t="s">
+      <c r="E8" s="18"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="8">
         <v>3</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="8">
         <v>3</v>
       </c>
-      <c r="M8" s="28" t="s">
+      <c r="M8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="8">
         <v>3</v>
       </c>
-      <c r="O8" s="28" t="s">
+      <c r="O8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="61">
+      <c r="P8" s="41">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21">
+      <c r="A9" s="8">
         <v>4</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="33" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="35" t="s">
+      <c r="E9" s="21"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="8">
         <v>4</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="L9" s="21">
+      <c r="L9" s="8">
         <v>4</v>
       </c>
-      <c r="M9" s="28" t="s">
+      <c r="M9" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="8">
         <v>4</v>
       </c>
-      <c r="O9" s="28" t="s">
+      <c r="O9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="P9" s="61">
+      <c r="P9" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="8">
         <v>5</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37" t="s">
+      <c r="C10" s="10"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F10" s="26"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="37" t="s">
+      <c r="F10" s="13"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="8">
         <v>5</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="8">
         <v>5</v>
       </c>
-      <c r="M10" s="28" t="s">
+      <c r="M10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="8">
         <v>5</v>
       </c>
-      <c r="O10" s="28" t="s">
+      <c r="O10" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="P10" s="61">
+      <c r="P10" s="41">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21">
+      <c r="A11" s="8">
         <v>6</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="32" t="s">
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="38" t="s">
+      <c r="F11" s="13"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="21">
+      <c r="J11" s="8">
         <v>6</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="21">
+      <c r="L11" s="8">
         <v>6</v>
       </c>
-      <c r="M11" s="28" t="s">
+      <c r="M11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="8">
         <v>6</v>
       </c>
-      <c r="O11" s="28" t="s">
+      <c r="O11" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="P11" s="61">
+      <c r="P11" s="41">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
+      <c r="A12" s="8">
         <v>7</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="35" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="39" t="s">
+      <c r="F12" s="13"/>
+      <c r="G12" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="H12" s="31"/>
-      <c r="J12" s="21">
+      <c r="H12" s="18"/>
+      <c r="J12" s="8">
         <v>7</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="8">
         <v>7</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="N12" s="21">
+      <c r="N12" s="8">
         <v>7</v>
       </c>
-      <c r="O12" s="28" t="s">
+      <c r="O12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="P12" s="61">
+      <c r="P12" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21">
+      <c r="A13" s="8">
         <v>8</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="25" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="42"/>
-      <c r="J13" s="21">
+      <c r="H13" s="29"/>
+      <c r="J13" s="8">
         <v>8</v>
       </c>
-      <c r="K13" s="22" t="s">
+      <c r="K13" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="L13" s="21">
+      <c r="L13" s="8">
         <v>8</v>
       </c>
-      <c r="M13" s="28" t="s">
+      <c r="M13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="N13" s="43">
+      <c r="N13" s="30">
         <v>8</v>
       </c>
-      <c r="O13" s="57" t="s">
+      <c r="O13" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="P13" s="62">
+      <c r="P13" s="42">
         <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21">
+      <c r="A14" s="8">
         <v>9</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="38" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="26"/>
-      <c r="G14" s="30" t="s">
+      <c r="F14" s="13"/>
+      <c r="G14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="42"/>
-      <c r="J14" s="21">
+      <c r="H14" s="29"/>
+      <c r="J14" s="8">
         <v>9</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="K14" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="8">
         <v>9</v>
       </c>
-      <c r="M14" s="22" t="s">
+      <c r="M14" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21">
+      <c r="A15" s="8">
         <v>10</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="39" t="s">
+      <c r="C15" s="10"/>
+      <c r="D15" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="27" t="s">
+      <c r="E15" s="18"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="H15" s="42"/>
-      <c r="J15" s="21">
+      <c r="H15" s="29"/>
+      <c r="J15" s="8">
         <v>10</v>
       </c>
-      <c r="K15" s="22" t="s">
+      <c r="K15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="21">
+      <c r="L15" s="8">
         <v>10</v>
       </c>
-      <c r="M15" s="22" t="s">
+      <c r="M15" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
     </row>
     <row r="16" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="8">
         <v>11</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="38" t="s">
+      <c r="C16" s="10"/>
+      <c r="D16" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="42"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="37" t="s">
+      <c r="E16" s="29"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="42"/>
-      <c r="J16" s="21">
+      <c r="H16" s="29"/>
+      <c r="J16" s="8">
         <v>11</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="L16" s="21">
+      <c r="L16" s="8">
         <v>11</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
     </row>
     <row r="17" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21">
+      <c r="A17" s="8">
         <v>12</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="45" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="38" t="s">
+      <c r="E17" s="21"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="42"/>
-      <c r="J17" s="21">
+      <c r="H17" s="29"/>
+      <c r="J17" s="8">
         <v>12</v>
       </c>
-      <c r="K17" s="22" t="s">
+      <c r="K17" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="L17" s="21">
+      <c r="L17" s="8">
         <v>12</v>
       </c>
-      <c r="M17" s="22" t="s">
+      <c r="M17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
     </row>
     <row r="18" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21">
+      <c r="A18" s="8">
         <v>13</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="45" t="s">
+      <c r="C18" s="10"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="45" t="s">
+      <c r="F18" s="13"/>
+      <c r="G18" s="32" t="s">
         <v>75</v>
       </c>
-      <c r="H18" s="34"/>
-      <c r="J18" s="21">
+      <c r="H18" s="21"/>
+      <c r="J18" s="8">
         <v>13</v>
       </c>
-      <c r="K18" s="22" t="s">
+      <c r="K18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="L18" s="21">
+      <c r="L18" s="8">
         <v>13</v>
       </c>
-      <c r="M18" s="22" t="s">
+      <c r="M18" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
     </row>
     <row r="19" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21">
+      <c r="A19" s="8">
         <v>14</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="30" t="s">
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="26"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="33" t="s">
+      <c r="F19" s="13"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="8">
         <v>14</v>
       </c>
-      <c r="K19" s="22" t="s">
+      <c r="K19" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="L19" s="21">
+      <c r="L19" s="8">
         <v>14</v>
       </c>
-      <c r="M19" s="22" t="s">
+      <c r="M19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
     </row>
     <row r="20" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21">
+      <c r="A20" s="8">
         <v>15</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="30" t="s">
+      <c r="C20" s="10"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="8">
         <v>15</v>
       </c>
-      <c r="K20" s="22" t="s">
+      <c r="K20" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="L20" s="21">
+      <c r="L20" s="8">
         <v>15</v>
       </c>
-      <c r="M20" s="22" t="s">
+      <c r="M20" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
     </row>
     <row r="21" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21">
+      <c r="A21" s="8">
         <v>16</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="33" t="s">
+      <c r="C21" s="10"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="26"/>
-      <c r="G21" s="33" t="s">
+      <c r="F21" s="13"/>
+      <c r="G21" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="H21" s="31"/>
-      <c r="J21" s="21">
+      <c r="H21" s="18"/>
+      <c r="J21" s="8">
         <v>16</v>
       </c>
-      <c r="K21" s="22" t="s">
+      <c r="K21" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="L21" s="21">
+      <c r="L21" s="8">
         <v>16</v>
       </c>
-      <c r="M21" s="22" t="s">
+      <c r="M21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
     </row>
     <row r="22" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21">
+      <c r="A22" s="8">
         <v>17</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="37" t="s">
+      <c r="C22" s="10"/>
+      <c r="D22" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="32" t="s">
+      <c r="E22" s="18"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="H22" s="42"/>
-      <c r="J22" s="21">
+      <c r="H22" s="29"/>
+      <c r="J22" s="8">
         <v>17</v>
       </c>
-      <c r="K22" s="22" t="s">
+      <c r="K22" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="L22" s="21">
+      <c r="L22" s="8">
         <v>17</v>
       </c>
-      <c r="M22" s="22" t="s">
+      <c r="M22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
     </row>
     <row r="23" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="21">
+      <c r="A23" s="8">
         <v>18</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="32" t="s">
+      <c r="C23" s="10"/>
+      <c r="D23" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="47"/>
-      <c r="J23" s="43">
+      <c r="E23" s="29"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="34"/>
+      <c r="J23" s="30">
         <v>18</v>
       </c>
-      <c r="K23" s="44"/>
-      <c r="L23" s="21">
+      <c r="K23" s="31"/>
+      <c r="L23" s="8">
         <v>18</v>
       </c>
-      <c r="M23" s="22" t="s">
+      <c r="M23" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
     </row>
     <row r="24" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21">
+      <c r="A24" s="8">
         <v>19</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="27" t="s">
+      <c r="C24" s="10"/>
+      <c r="D24" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="47"/>
-      <c r="J24" s="23"/>
-      <c r="K24" s="23"/>
-      <c r="L24" s="21">
+      <c r="E24" s="29"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="34"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="8">
         <v>19</v>
       </c>
-      <c r="M24" s="22" t="s">
+      <c r="M24" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
     </row>
     <row r="25" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="43">
+      <c r="A25" s="30">
         <v>20</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="25" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="48"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="50"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="23"/>
-      <c r="L25" s="51">
+      <c r="E25" s="35"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="38">
         <v>20</v>
       </c>
-      <c r="M25" s="22" t="s">
+      <c r="M25" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="21">
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="8">
         <v>21</v>
       </c>
-      <c r="M26" s="22" t="s">
+      <c r="M26" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L27" s="21">
+      <c r="L27" s="8">
         <v>22</v>
       </c>
-      <c r="M27" s="22" t="s">
+      <c r="M27" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L28" s="21">
+      <c r="L28" s="8">
         <v>23</v>
       </c>
-      <c r="M28" s="22" t="s">
+      <c r="M28" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L29" s="21">
+      <c r="L29" s="8">
         <v>24</v>
       </c>
-      <c r="M29" s="22" t="s">
+      <c r="M29" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L30" s="21">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L30" s="8">
         <v>25</v>
       </c>
-      <c r="M30" s="22" t="s">
+      <c r="M30" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L31" s="21">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="L31" s="8">
         <v>26</v>
       </c>
-      <c r="M31" s="22" t="s">
+      <c r="M31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O31" s="52"/>
-      <c r="P31" s="23"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L32" s="21">
+      <c r="L32" s="8">
         <v>27</v>
       </c>
-      <c r="M32" s="22" t="s">
+      <c r="M32" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="33" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L33" s="21">
+      <c r="L33" s="8">
         <v>28</v>
       </c>
-      <c r="M33" s="22" t="s">
+      <c r="M33" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="34" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L34" s="21">
+      <c r="L34" s="8">
         <v>29</v>
       </c>
-      <c r="M34" s="22" t="s">
+      <c r="M34" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L35" s="21">
+      <c r="L35" s="8">
         <v>30</v>
       </c>
-      <c r="M35" s="22" t="s">
+      <c r="M35" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="36" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L36" s="21">
+      <c r="L36" s="8">
         <v>31</v>
       </c>
-      <c r="M36" s="22" t="s">
+      <c r="M36" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L37" s="21">
+      <c r="L37" s="8">
         <v>32</v>
       </c>
-      <c r="M37" s="22" t="s">
+      <c r="M37" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L38" s="21">
+      <c r="L38" s="8">
         <v>33</v>
       </c>
-      <c r="M38" s="22" t="s">
+      <c r="M38" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="39" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L39" s="21">
+      <c r="L39" s="8">
         <v>34</v>
       </c>
-      <c r="M39" s="22" t="s">
+      <c r="M39" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="40" spans="12:13" x14ac:dyDescent="0.2">
-      <c r="L40" s="21">
+      <c r="L40" s="8">
         <v>35</v>
       </c>
-      <c r="M40" s="22" t="s">
+      <c r="M40" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="41" spans="12:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L41" s="43">
+      <c r="L41" s="30">
         <v>36</v>
       </c>
-      <c r="M41" s="44" t="s">
+      <c r="M41" s="31" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N4:P4"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="A2:B2"/>
@@ -2642,6 +2635,12 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="D4:E4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N4:P4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>